<commit_message>
added a middle name in excel file
</commit_message>
<xml_diff>
--- a/GitHub Info sans duplicates.xlsx
+++ b/GitHub Info sans duplicates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Houdin\staffcard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\staffcard\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9795CA07-9D82-4C0D-89FD-F4DDFBC785C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3294" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3294" uniqueCount="907">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2744,12 +2745,15 @@
   </si>
   <si>
     <t>255757463345</t>
+  </si>
+  <si>
+    <t>DANIEL SOLOMON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yyyy"/>
@@ -3227,12 +3231,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C94" sqref="C94"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8032,135 +8036,135 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-    <hyperlink ref="L5" r:id="rId4"/>
-    <hyperlink ref="L6" r:id="rId5"/>
-    <hyperlink ref="L7" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
-    <hyperlink ref="L9" r:id="rId8"/>
-    <hyperlink ref="L10" r:id="rId9"/>
-    <hyperlink ref="L11" r:id="rId10"/>
-    <hyperlink ref="L12" r:id="rId11"/>
-    <hyperlink ref="L13" r:id="rId12"/>
-    <hyperlink ref="L14" r:id="rId13"/>
-    <hyperlink ref="L15" r:id="rId14"/>
-    <hyperlink ref="L16" r:id="rId15"/>
-    <hyperlink ref="L17" r:id="rId16"/>
-    <hyperlink ref="L18" r:id="rId17"/>
-    <hyperlink ref="L19" r:id="rId18"/>
-    <hyperlink ref="L20" r:id="rId19"/>
-    <hyperlink ref="L21" r:id="rId20"/>
-    <hyperlink ref="L22" r:id="rId21"/>
-    <hyperlink ref="L23" r:id="rId22"/>
-    <hyperlink ref="L24" r:id="rId23"/>
-    <hyperlink ref="L25" r:id="rId24"/>
-    <hyperlink ref="L26" r:id="rId25"/>
-    <hyperlink ref="L27" r:id="rId26"/>
-    <hyperlink ref="L28" r:id="rId27"/>
-    <hyperlink ref="L29" r:id="rId28"/>
-    <hyperlink ref="L30" r:id="rId29"/>
-    <hyperlink ref="L31" r:id="rId30"/>
-    <hyperlink ref="L32" r:id="rId31"/>
-    <hyperlink ref="L33" r:id="rId32"/>
-    <hyperlink ref="L34" r:id="rId33"/>
-    <hyperlink ref="L35" r:id="rId34"/>
-    <hyperlink ref="L36" r:id="rId35"/>
-    <hyperlink ref="L37" r:id="rId36"/>
-    <hyperlink ref="L38" r:id="rId37"/>
-    <hyperlink ref="L39" r:id="rId38"/>
-    <hyperlink ref="L40" r:id="rId39"/>
-    <hyperlink ref="L41" r:id="rId40"/>
-    <hyperlink ref="L42" r:id="rId41"/>
-    <hyperlink ref="L43" r:id="rId42"/>
-    <hyperlink ref="L44" r:id="rId43"/>
-    <hyperlink ref="L45" r:id="rId44"/>
-    <hyperlink ref="L46" r:id="rId45"/>
-    <hyperlink ref="L47" r:id="rId46"/>
-    <hyperlink ref="L48" r:id="rId47"/>
-    <hyperlink ref="L49" r:id="rId48"/>
-    <hyperlink ref="L50" r:id="rId49"/>
-    <hyperlink ref="L51" r:id="rId50"/>
-    <hyperlink ref="L52" r:id="rId51"/>
-    <hyperlink ref="L53" r:id="rId52"/>
-    <hyperlink ref="L54" r:id="rId53"/>
-    <hyperlink ref="L55" r:id="rId54"/>
-    <hyperlink ref="L56" r:id="rId55"/>
-    <hyperlink ref="L57" r:id="rId56"/>
-    <hyperlink ref="L58" r:id="rId57"/>
-    <hyperlink ref="L59" r:id="rId58"/>
-    <hyperlink ref="L60" r:id="rId59"/>
-    <hyperlink ref="L61" r:id="rId60"/>
-    <hyperlink ref="L62" r:id="rId61"/>
-    <hyperlink ref="L63" r:id="rId62"/>
-    <hyperlink ref="L64" r:id="rId63"/>
-    <hyperlink ref="L65" r:id="rId64"/>
-    <hyperlink ref="L66" r:id="rId65"/>
-    <hyperlink ref="L67" r:id="rId66"/>
-    <hyperlink ref="L68" r:id="rId67"/>
-    <hyperlink ref="L69" r:id="rId68"/>
-    <hyperlink ref="L70" r:id="rId69"/>
-    <hyperlink ref="L71" r:id="rId70"/>
-    <hyperlink ref="L72" r:id="rId71"/>
-    <hyperlink ref="L73" r:id="rId72"/>
-    <hyperlink ref="L74" r:id="rId73"/>
-    <hyperlink ref="L75" r:id="rId74"/>
-    <hyperlink ref="L76" r:id="rId75"/>
-    <hyperlink ref="L77" r:id="rId76"/>
-    <hyperlink ref="L78" r:id="rId77"/>
-    <hyperlink ref="L79" r:id="rId78"/>
-    <hyperlink ref="L80" r:id="rId79"/>
-    <hyperlink ref="L81" r:id="rId80"/>
-    <hyperlink ref="L82" r:id="rId81"/>
-    <hyperlink ref="L83" r:id="rId82"/>
-    <hyperlink ref="L84" r:id="rId83"/>
-    <hyperlink ref="L85" r:id="rId84"/>
-    <hyperlink ref="L86" r:id="rId85"/>
-    <hyperlink ref="L87" r:id="rId86"/>
-    <hyperlink ref="L88" r:id="rId87"/>
-    <hyperlink ref="L89" r:id="rId88"/>
-    <hyperlink ref="L90" r:id="rId89"/>
-    <hyperlink ref="L91" r:id="rId90"/>
-    <hyperlink ref="L92" r:id="rId91"/>
-    <hyperlink ref="L93" r:id="rId92"/>
-    <hyperlink ref="L94" r:id="rId93"/>
-    <hyperlink ref="L95" r:id="rId94"/>
-    <hyperlink ref="L96" r:id="rId95"/>
-    <hyperlink ref="L97" r:id="rId96"/>
-    <hyperlink ref="L98" r:id="rId97"/>
-    <hyperlink ref="L99" r:id="rId98"/>
-    <hyperlink ref="L100" r:id="rId99"/>
-    <hyperlink ref="L101" r:id="rId100"/>
-    <hyperlink ref="L102" r:id="rId101"/>
-    <hyperlink ref="L103" r:id="rId102"/>
-    <hyperlink ref="L104" r:id="rId103"/>
-    <hyperlink ref="L105" r:id="rId104"/>
-    <hyperlink ref="L106" r:id="rId105"/>
-    <hyperlink ref="L107" r:id="rId106"/>
-    <hyperlink ref="L108" r:id="rId107"/>
-    <hyperlink ref="L109" r:id="rId108"/>
-    <hyperlink ref="L110" r:id="rId109"/>
-    <hyperlink ref="L111" r:id="rId110"/>
-    <hyperlink ref="L112" r:id="rId111"/>
-    <hyperlink ref="L113" r:id="rId112"/>
-    <hyperlink ref="L114" r:id="rId113"/>
-    <hyperlink ref="L115" r:id="rId114"/>
-    <hyperlink ref="L116" r:id="rId115"/>
-    <hyperlink ref="L117" r:id="rId116"/>
-    <hyperlink ref="L118" r:id="rId117"/>
-    <hyperlink ref="L119" r:id="rId118"/>
-    <hyperlink ref="L120" r:id="rId119"/>
-    <hyperlink ref="L121" r:id="rId120"/>
-    <hyperlink ref="L122" r:id="rId121"/>
-    <hyperlink ref="G123" r:id="rId122"/>
-    <hyperlink ref="L123" r:id="rId123"/>
-    <hyperlink ref="G124" r:id="rId124"/>
-    <hyperlink ref="L124" r:id="rId125"/>
-    <hyperlink ref="G125" r:id="rId126"/>
-    <hyperlink ref="G126" r:id="rId127"/>
-    <hyperlink ref="G127" r:id="rId128"/>
-    <hyperlink ref="L127" r:id="rId129"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="L10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="L11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="L12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="L13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="L14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="L15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="L16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="L17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="L18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="L19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="L27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="L30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="L33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="L35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="L38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="L39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="L40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="L41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="L42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="L43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="L44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="L45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="L46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="L47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="L49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="L50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="L51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="L52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="L53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="L54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="L55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="L56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="L57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="L58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="L59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="L60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="L61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="L62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="L63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="L64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="L65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="L66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="L67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="L68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="L69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="L70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="L71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="L72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="L73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="L74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="L75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="L76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="L77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="L78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="L79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="L80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="L81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="L82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="L83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="L84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="L85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="L86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="L87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="L88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="L89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="L90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="L91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="L92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="L93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="L94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="L95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="L96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="L97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="L98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="L99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="L100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="L101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="L102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="L103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="L104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="L105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="L106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="L107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="L108" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="L109" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="L110" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="L111" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="L112" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="L113" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="L114" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="L115" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="L116" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="L117" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="L118" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="L119" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="L120" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="L121" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="L122" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="G123" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="L123" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="G124" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="L124" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="G125" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="G126" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="G127" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="L127" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8168,14 +8172,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P212"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
     </sheetView>
@@ -12170,121 +12174,121 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
-    <hyperlink ref="J110" r:id="rId109"/>
-    <hyperlink ref="J111" r:id="rId110"/>
-    <hyperlink ref="J112" r:id="rId111"/>
-    <hyperlink ref="J113" r:id="rId112"/>
-    <hyperlink ref="J114" r:id="rId113"/>
-    <hyperlink ref="G115" r:id="rId114"/>
-    <hyperlink ref="J115" r:id="rId115"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="J111" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="J112" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="J113" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="J114" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="G115" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="J115" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -12293,15 +12297,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P198"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13488,7 +13492,7 @@
         <v>311</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>312</v>
+        <v>906</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>313</v>
@@ -16165,119 +16169,119 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
-    <hyperlink ref="G110" r:id="rId109"/>
-    <hyperlink ref="J110" r:id="rId110"/>
-    <hyperlink ref="G111" r:id="rId111"/>
-    <hyperlink ref="J111" r:id="rId112"/>
-    <hyperlink ref="G112" r:id="rId113"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0200-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0200-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0200-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0200-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0200-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0200-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0200-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0200-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0200-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0200-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0200-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0200-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0200-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0200-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0200-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0200-00006B000000}"/>
+    <hyperlink ref="G110" r:id="rId109" xr:uid="{00000000-0004-0000-0200-00006C000000}"/>
+    <hyperlink ref="J110" r:id="rId110" xr:uid="{00000000-0004-0000-0200-00006D000000}"/>
+    <hyperlink ref="G111" r:id="rId111" xr:uid="{00000000-0004-0000-0200-00006E000000}"/>
+    <hyperlink ref="J111" r:id="rId112" xr:uid="{00000000-0004-0000-0200-00006F000000}"/>
+    <hyperlink ref="G112" r:id="rId113" xr:uid="{00000000-0004-0000-0200-000070000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>